<commit_message>
update db and sample data
</commit_message>
<xml_diff>
--- a/excel_student/test.xlsx
+++ b/excel_student/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>รหัสนักศึกษา</t>
   </si>
@@ -30,25 +30,73 @@
     <t>นามสกุล</t>
   </si>
   <si>
-    <t>ทดสอบ</t>
-  </si>
-  <si>
-    <t>ลองดู</t>
-  </si>
-  <si>
-    <t>ลองดู6767</t>
-  </si>
-  <si>
     <t>รายชื่อผู้ร่วมเดินทาง</t>
   </si>
   <si>
     <t>หมายเหตุ</t>
   </si>
   <si>
-    <t>ลองดูok</t>
-  </si>
-  <si>
-    <t>โทร.0899454565464</t>
+    <t>6110620013</t>
+  </si>
+  <si>
+    <t>6110620033</t>
+  </si>
+  <si>
+    <t>6110620034</t>
+  </si>
+  <si>
+    <t>6110620035</t>
+  </si>
+  <si>
+    <t>6110620038</t>
+  </si>
+  <si>
+    <t>6110620045</t>
+  </si>
+  <si>
+    <t>6110620048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">น.ส. ฐิตาภรณ์ </t>
+  </si>
+  <si>
+    <t>อนุสาร</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นาย กิตตินันท์ </t>
+  </si>
+  <si>
+    <t>ขวัญซ้าย</t>
+  </si>
+  <si>
+    <t xml:space="preserve">น.ส. เขมินี </t>
+  </si>
+  <si>
+    <t>ทองมา</t>
+  </si>
+  <si>
+    <t xml:space="preserve">น.ส. จอมทอง </t>
+  </si>
+  <si>
+    <t>ชัยภักดี</t>
+  </si>
+  <si>
+    <t xml:space="preserve">น.ส. ทิพยเนตร </t>
+  </si>
+  <si>
+    <t>จงจิตร</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นาย พีระพัฒน์ </t>
+  </si>
+  <si>
+    <t>เพ่งพิศ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">น.ส. สุชานาถ </t>
+  </si>
+  <si>
+    <t>กองวารี</t>
   </si>
 </sst>
 </file>
@@ -375,26 +423,26 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" customWidth="1"/>
-    <col min="3" max="3" width="22.296875" customWidth="1"/>
-    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.75" customWidth="1"/>
+    <col min="3" max="3" width="22.25" customWidth="1"/>
+    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -405,87 +453,84 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>56123456678</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>56123456679</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>56123456680</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>56123456681</v>
-      </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>56123456682</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>56123456683</v>
-      </c>
-      <c r="B8" s="1">
-        <v>555</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>56123456684</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>